<commit_message>
-Added Haunted Carriage info, removed some redundant code.
</commit_message>
<xml_diff>
--- a/DI_Timer_App/DI_Lookup_Table.xlsx
+++ b/DI_Timer_App/DI_Lookup_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\DI_Timer_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB5B45F-597F-45CF-9DDF-16742D68A330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBD740A-31DE-476D-ADB6-7535CF74B38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35370" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Server_Name</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>EDT</t>
+  </si>
+  <si>
+    <t>Haunted_Carriage_12PM</t>
+  </si>
+  <si>
+    <t>Haunted_Carriage_830PM</t>
+  </si>
+  <si>
+    <t>Haunted_Carriage_10PM</t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7687A13-5412-415C-B505-B9EB7AB383A0}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,9 +461,12 @@
     <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +497,17 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -500,7 +521,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
-Added Ancient Arena timer logic.
</commit_message>
<xml_diff>
--- a/DI_Timer_App/DI_Lookup_Table.xlsx
+++ b/DI_Timer_App/DI_Lookup_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\DI_Timer_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EFFC59-02A4-4AC0-9D05-D5E9D00D9806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B874D1-1DDE-4DCA-9811-7B257EF29C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34080" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Server_Name</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Demon_Gates_10PM</t>
+  </si>
+  <si>
+    <t>Ancient_Arena_930PM</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7687A13-5412-415C-B505-B9EB7AB383A0}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:P1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,9 +478,10 @@
     <col min="13" max="14" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,8 +530,11 @@
       <c r="P1" t="s">
         <v>21</v>
       </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -541,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>

</xml_diff>